<commit_message>
Increased the figures for videos and AdWords and took out direct mail altogether.
</commit_message>
<xml_diff>
--- a/Excel/Marketing Budget.xlsx
+++ b/Excel/Marketing Budget.xlsx
@@ -74,15 +74,6 @@
     <t>Print</t>
   </si>
   <si>
-    <t>Radio</t>
-  </si>
-  <si>
-    <t>Television</t>
-  </si>
-  <si>
-    <t>Direct Mail</t>
-  </si>
-  <si>
     <t>Point of Purchase</t>
   </si>
   <si>
@@ -153,6 +144,15 @@
   </si>
   <si>
     <t>Grand Totals</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Ad-Words</t>
   </si>
 </sst>
 </file>
@@ -934,7 +934,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
@@ -984,6 +984,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="52" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="75">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1543,7 +1544,7 @@
   <dimension ref="B3:J52"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1635,8 +1636,8 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>8</v>
+      <c r="B7" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="C7" s="10">
         <v>10000</v>
@@ -1668,8 +1669,8 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>9</v>
+      <c r="B8" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="C8" s="12">
         <v>10000</v>
@@ -1701,8 +1702,8 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
+      <c r="B9" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="12">
         <v>25000</v>
@@ -1734,8 +1735,8 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
-        <v>11</v>
+      <c r="B10" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="C10" s="12">
         <v>30000</v>
@@ -1768,7 +1769,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11" s="12">
         <v>5000</v>
@@ -1801,7 +1802,7 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C12" s="12">
         <v>5000</v>
@@ -1834,7 +1835,7 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13" s="14">
         <v>1000</v>
@@ -1867,7 +1868,7 @@
     </row>
     <row r="14" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C14" s="16">
         <f>IF(SUM(C7:C13),SUM(C7:C13),"")</f>
@@ -1875,7 +1876,7 @@
       </c>
       <c r="D14" s="17">
         <f>IF(SUM(C7:C13),C14/C49,"")</f>
-        <v>0.12044817927170869</v>
+        <v>0.11894882434301521</v>
       </c>
       <c r="E14" s="16">
         <f>IF(SUM(E7:E13),SUM(E7:E13),"")</f>
@@ -1883,7 +1884,7 @@
       </c>
       <c r="F14" s="17">
         <f>IF(SUM(E7:E13),E14/E49,"")</f>
-        <v>0.13099257258609048</v>
+        <v>0.12941961307538358</v>
       </c>
       <c r="G14" s="16">
         <f>IF(SUM(G7:G13),SUM(G7:G13),"")</f>
@@ -1891,7 +1892,7 @@
       </c>
       <c r="H14" s="17">
         <f>IF(SUM(G7:G13),G14/G49,"")</f>
-        <v>0.12044817927170869</v>
+        <v>0.11894882434301521</v>
       </c>
       <c r="I14" s="16">
         <f>IF(SUM(I7:I13),SUM(I7:I13),"")</f>
@@ -1899,12 +1900,12 @@
       </c>
       <c r="J14" s="17">
         <f>IF(SUM(I7:I13),I14/I49,"")</f>
-        <v>0.13099257258609048</v>
+        <v>0.12941961307538358</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -1917,7 +1918,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C16" s="10">
         <v>2000</v>
@@ -1950,7 +1951,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C17" s="12">
         <v>10000</v>
@@ -1983,7 +1984,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18" s="14">
         <v>1000</v>
@@ -2016,7 +2017,7 @@
     </row>
     <row r="19" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" s="16">
         <f>IF(SUM(C16:C18),SUM(C16:C18),"")</f>
@@ -2024,7 +2025,7 @@
       </c>
       <c r="D19" s="17">
         <f>IF(SUM(C16:C18),+C19/C49,"")</f>
-        <v>1.8207282913165267E-2</v>
+        <v>1.7980636237897647E-2</v>
       </c>
       <c r="E19" s="16">
         <f>IF(SUM(E16:E18),SUM(E16:E18),"")</f>
@@ -2032,7 +2033,7 @@
       </c>
       <c r="F19" s="17">
         <f>IF(SUM(E16:E18),+E19/E49,"")</f>
-        <v>7.4274139095205942E-3</v>
+        <v>7.3382254836557703E-3</v>
       </c>
       <c r="G19" s="16">
         <f>IF(SUM(G16:G18),SUM(G16:G18),"")</f>
@@ -2040,7 +2041,7 @@
       </c>
       <c r="H19" s="17">
         <f>IF(SUM(G16:G18),+G19/G49,"")</f>
-        <v>1.8207282913165267E-2</v>
+        <v>1.7980636237897647E-2</v>
       </c>
       <c r="I19" s="16">
         <f>IF(SUM(I16:I18),SUM(I16:I18),"")</f>
@@ -2048,12 +2049,12 @@
       </c>
       <c r="J19" s="17">
         <f>IF(SUM(I16:I18),+I19/I49,"")</f>
-        <v>7.4274139095205942E-3</v>
+        <v>7.3382254836557703E-3</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
@@ -2066,7 +2067,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C21" s="10">
         <v>100000</v>
@@ -2099,7 +2100,7 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C22" s="12">
         <v>200000</v>
@@ -2132,7 +2133,7 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C23" s="12">
         <v>40000</v>
@@ -2165,7 +2166,7 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C24" s="12">
         <v>15000</v>
@@ -2198,7 +2199,7 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C25" s="12">
         <v>8000</v>
@@ -2231,7 +2232,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C26" s="14">
         <v>1000</v>
@@ -2264,7 +2265,7 @@
     </row>
     <row r="27" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C27" s="16">
         <f>IF(SUM(C21:C26),SUM(C21:C26),"")</f>
@@ -2272,7 +2273,7 @@
       </c>
       <c r="D27" s="17">
         <f>IF(SUM(C21:C26),C27/C49,"")</f>
-        <v>0.50980392156862742</v>
+        <v>0.50345781466113415</v>
       </c>
       <c r="E27" s="16">
         <f>IF(SUM(E21:E26),SUM(E21:E26),"")</f>
@@ -2280,7 +2281,7 @@
       </c>
       <c r="F27" s="17">
         <f>IF(SUM(E21:E26),E27/E49,"")</f>
-        <v>0.52261985145172185</v>
+        <v>0.51634422948632419</v>
       </c>
       <c r="G27" s="16">
         <f>IF(SUM(G21:G26),SUM(G21:G26),"")</f>
@@ -2288,7 +2289,7 @@
       </c>
       <c r="H27" s="17">
         <f>IF(SUM(G21:G26),G27/G49,"")</f>
-        <v>0.50980392156862742</v>
+        <v>0.50345781466113415</v>
       </c>
       <c r="I27" s="16">
         <f>IF(SUM(I21:I26),SUM(I21:I26),"")</f>
@@ -2296,12 +2297,12 @@
       </c>
       <c r="J27" s="17">
         <f>IF(SUM(I21:I26),I27/I49,"")</f>
-        <v>0.52261985145172185</v>
+        <v>0.51634422948632419</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
@@ -2314,176 +2315,176 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C29" s="10">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="D29" s="11">
         <f>IF(SUM(C29:C32),+C29/C33,"")</f>
-        <v>2.7027027027027029E-2</v>
+        <v>0.21739130434782608</v>
       </c>
       <c r="E29" s="10">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="F29" s="11">
         <f>IF(SUM(E29:E32),+E29/E33,"")</f>
-        <v>2.7027027027027029E-2</v>
+        <v>0.21739130434782608</v>
       </c>
       <c r="G29" s="10">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H29" s="11">
         <f>IF(SUM(G29:G32),+G29/G33,"")</f>
-        <v>2.7027027027027029E-2</v>
+        <v>0.21739130434782608</v>
       </c>
       <c r="I29" s="10">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="J29" s="11">
         <f>IF(SUM(I29:I32),+I29/I33,"")</f>
-        <v>2.7027027027027029E-2</v>
+        <v>0.21739130434782608</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C30" s="12">
         <v>20000</v>
       </c>
       <c r="D30" s="11">
         <f>IF(SUM(C29:C32),+C30/C33,"")</f>
-        <v>0.54054054054054057</v>
+        <v>0.43478260869565216</v>
       </c>
       <c r="E30" s="12">
         <v>20000</v>
       </c>
       <c r="F30" s="11">
         <f>IF(SUM(E29:E32),+E30/E33,"")</f>
-        <v>0.54054054054054057</v>
+        <v>0.43478260869565216</v>
       </c>
       <c r="G30" s="12">
         <v>20000</v>
       </c>
       <c r="H30" s="11">
         <f>IF(SUM(G29:G32),+G30/G33,"")</f>
-        <v>0.54054054054054057</v>
+        <v>0.43478260869565216</v>
       </c>
       <c r="I30" s="12">
         <v>20000</v>
       </c>
       <c r="J30" s="11">
         <f>IF(SUM(I29:I32),+I30/I33,"")</f>
-        <v>0.54054054054054057</v>
+        <v>0.43478260869565216</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C31" s="12">
         <v>15000</v>
       </c>
       <c r="D31" s="11">
         <f>IF(SUM(C29:C32),+C31/C33,"")</f>
-        <v>0.40540540540540543</v>
+        <v>0.32608695652173914</v>
       </c>
       <c r="E31" s="12">
         <v>15000</v>
       </c>
       <c r="F31" s="11">
         <f>IF(SUM(E29:E32),+E31/E33,"")</f>
-        <v>0.40540540540540543</v>
+        <v>0.32608695652173914</v>
       </c>
       <c r="G31" s="12">
         <v>15000</v>
       </c>
       <c r="H31" s="11">
         <f>IF(SUM(G29:G32),+G31/G33,"")</f>
-        <v>0.40540540540540543</v>
+        <v>0.32608695652173914</v>
       </c>
       <c r="I31" s="12">
         <v>15000</v>
       </c>
       <c r="J31" s="11">
         <f>IF(SUM(I29:I32),+I31/I33,"")</f>
-        <v>0.40540540540540543</v>
+        <v>0.32608695652173914</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C32" s="14">
         <v>1000</v>
       </c>
       <c r="D32" s="15">
         <f>IF(SUM(C29:C32),+C32/C33,"")</f>
-        <v>2.7027027027027029E-2</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="E32" s="14">
         <v>1000</v>
       </c>
       <c r="F32" s="15">
         <f>IF(SUM(E29:E32),+E32/E33,"")</f>
-        <v>2.7027027027027029E-2</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="G32" s="14">
         <v>1000</v>
       </c>
       <c r="H32" s="15">
         <f>IF(SUM(G29:G32),+G32/G33,"")</f>
-        <v>2.7027027027027029E-2</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="I32" s="14">
         <v>1000</v>
       </c>
       <c r="J32" s="15">
         <f>IF(SUM(I29:I32),+I32/I33,"")</f>
-        <v>2.7027027027027029E-2</v>
+        <v>2.1739130434782608E-2</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C33" s="16">
         <f>IF(SUM(C29:C32),SUM(C29:C32),"")</f>
-        <v>37000</v>
+        <v>46000</v>
       </c>
       <c r="D33" s="17">
         <f>IF(SUM(C29:C32),+C33/C49,"")</f>
-        <v>5.182072829131653E-2</v>
+        <v>6.3623789764868599E-2</v>
       </c>
       <c r="E33" s="16">
         <f>IF(SUM(E29:E32),SUM(E29:E32),"")</f>
-        <v>37000</v>
+        <v>46000</v>
       </c>
       <c r="F33" s="17">
         <f>IF(SUM(E29:E32),+E33/E49,"")</f>
-        <v>4.9966239027683997E-2</v>
+        <v>6.1374249499666446E-2</v>
       </c>
       <c r="G33" s="16">
         <f>IF(SUM(G29:G32),SUM(G29:G32),"")</f>
-        <v>37000</v>
+        <v>46000</v>
       </c>
       <c r="H33" s="17">
         <f>IF(SUM(G29:G32),+G33/G49,"")</f>
-        <v>5.182072829131653E-2</v>
+        <v>6.3623789764868599E-2</v>
       </c>
       <c r="I33" s="16">
         <f>IF(SUM(I29:I32),SUM(I29:I32),"")</f>
-        <v>37000</v>
+        <v>46000</v>
       </c>
       <c r="J33" s="17">
         <f>IF(SUM(I29:I32),+I33/I49,"")</f>
-        <v>4.9966239027683997E-2</v>
+        <v>6.1374249499666446E-2</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -2496,7 +2497,7 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C35" s="10">
         <v>1000</v>
@@ -2529,7 +2530,7 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C36" s="12">
         <v>2000</v>
@@ -2562,7 +2563,7 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C37" s="12">
         <v>150000</v>
@@ -2595,7 +2596,7 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C38" s="12">
         <v>20000</v>
@@ -2628,7 +2629,7 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C39" s="12">
         <v>10000</v>
@@ -2661,7 +2662,7 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C40" s="14">
         <v>1000</v>
@@ -2694,7 +2695,7 @@
     </row>
     <row r="41" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C41" s="16">
         <f>IF(SUM(C35:C40),SUM(C35:C40),"")</f>
@@ -2702,7 +2703,7 @@
       </c>
       <c r="D41" s="17">
         <f>IF(SUM(C35:C40),+C41/C49,"")</f>
-        <v>0.25770308123249297</v>
+        <v>0.2544951590594744</v>
       </c>
       <c r="E41" s="16">
         <f>IF(SUM(E35:E40),SUM(E35:E40),"")</f>
@@ -2710,7 +2711,7 @@
       </c>
       <c r="F41" s="17">
         <f>IF(SUM(E35:E40),+E41/E49,"")</f>
-        <v>0.24848075624577987</v>
+        <v>0.24549699799866578</v>
       </c>
       <c r="G41" s="16">
         <f>IF(SUM(G35:G40),SUM(G35:G40),"")</f>
@@ -2718,7 +2719,7 @@
       </c>
       <c r="H41" s="17">
         <f>IF(SUM(G35:G40),+G41/G49,"")</f>
-        <v>0.25770308123249297</v>
+        <v>0.2544951590594744</v>
       </c>
       <c r="I41" s="16">
         <f>IF(SUM(I35:I40),SUM(I35:I40),"")</f>
@@ -2726,12 +2727,12 @@
       </c>
       <c r="J41" s="17">
         <f>IF(SUM(I35:I40),+I41/I49,"")</f>
-        <v>0.24848075624577987</v>
+        <v>0.24549699799866578</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -2744,7 +2745,7 @@
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C43" s="10">
         <v>15000</v>
@@ -2777,7 +2778,7 @@
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C44" s="12">
         <v>5000</v>
@@ -2810,7 +2811,7 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C45" s="12">
         <v>4000</v>
@@ -2843,7 +2844,7 @@
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C46" s="12">
         <v>5000</v>
@@ -2876,7 +2877,7 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C47" s="14">
         <v>1000</v>
@@ -2909,7 +2910,7 @@
     </row>
     <row r="48" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C48" s="16">
         <f>IF(SUM(C43:C47),SUM(C43:C47),"")</f>
@@ -2917,7 +2918,7 @@
       </c>
       <c r="D48" s="17">
         <f>IF(SUM(C43:C47),+C48/C49,"")</f>
-        <v>4.2016806722689079E-2</v>
+        <v>4.1493775933609957E-2</v>
       </c>
       <c r="E48" s="16">
         <f>IF(SUM(E43:E47),SUM(E43:E47),"")</f>
@@ -2925,7 +2926,7 @@
       </c>
       <c r="F48" s="17">
         <f>IF(SUM(E43:E47),+E48/E49,"")</f>
-        <v>4.051316677920324E-2</v>
+        <v>4.0026684456304203E-2</v>
       </c>
       <c r="G48" s="16">
         <f>IF(SUM(G43:G47),SUM(G43:G47),"")</f>
@@ -2933,7 +2934,7 @@
       </c>
       <c r="H48" s="17">
         <f>IF(SUM(G43:G47),+G48/G49,"")</f>
-        <v>4.2016806722689079E-2</v>
+        <v>4.1493775933609957E-2</v>
       </c>
       <c r="I48" s="16">
         <f>IF(SUM(I43:I47),SUM(I43:I47),"")</f>
@@ -2941,16 +2942,16 @@
       </c>
       <c r="J48" s="17">
         <f>IF(SUM(I43:I47),+I48/I49,"")</f>
-        <v>4.051316677920324E-2</v>
+        <v>4.0026684456304203E-2</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C49" s="16">
         <f>IF(SUM(C14,C19,C27,C33,C41),SUM(C14,C19,C27,C33,C41,C48),"")</f>
-        <v>714000</v>
+        <v>723000</v>
       </c>
       <c r="D49" s="19">
         <f>IF(SUM(C49),+C49/C49,"")</f>
@@ -2958,7 +2959,7 @@
       </c>
       <c r="E49" s="16">
         <f>IF(SUM(E14,E19,E27,E33,E41),SUM(E14,E19,E27,E33,E41,E48),"")</f>
-        <v>740500</v>
+        <v>749500</v>
       </c>
       <c r="F49" s="19">
         <f>IF(SUM(E49),+E49/E49,"")</f>
@@ -2966,7 +2967,7 @@
       </c>
       <c r="G49" s="16">
         <f>IF(SUM(G14,G19,G27,G33,G41),SUM(G14,G19,G27,G33,G41,G48),"")</f>
-        <v>714000</v>
+        <v>723000</v>
       </c>
       <c r="H49" s="19">
         <f>IF(SUM(G49),+G49/G49,"")</f>
@@ -2974,7 +2975,7 @@
       </c>
       <c r="I49" s="16">
         <f>IF(SUM(I14,I19,I27,I33,I41),SUM(I14,I19,I27,I33,I41,I48),"")</f>
-        <v>740500</v>
+        <v>749500</v>
       </c>
       <c r="J49" s="19">
         <f>IF(SUM(I49),+I49/I49,"")</f>

</xml_diff>

<commit_message>
Understood. I've cut back on travel for Q2 & Q3 , but if we need to go back we can revert to an earlier version easily enough.  Sound good?
</commit_message>
<xml_diff>
--- a/Excel/Marketing Budget.xlsx
+++ b/Excel/Marketing Budget.xlsx
@@ -978,13 +978,13 @@
     <xf numFmtId="0" fontId="36" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="52" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="52" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="75">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1544,7 +1544,7 @@
   <dimension ref="B3:J52"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1636,7 +1636,7 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="10">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="D7" s="11">
         <f>IF(SUM(C7:C13),+C7/C14,"")</f>
-        <v>0.11627906976744186</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="E7" s="10">
         <v>12000</v>
@@ -1669,15 +1669,15 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="12">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D8" s="11">
         <f>IF(SUM(C7:C13),+C8/C14,"")</f>
-        <v>0.11627906976744186</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="E8" s="12">
         <v>11000</v>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="12">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="D9" s="11">
         <f>IF(SUM(C7:C13),+C9/C14,"")</f>
-        <v>0.29069767441860467</v>
+        <v>0.26041666666666669</v>
       </c>
       <c r="E9" s="12">
         <v>28000</v>
@@ -1735,7 +1735,7 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="12">
@@ -1743,7 +1743,7 @@
       </c>
       <c r="D10" s="11">
         <f>IF(SUM(C7:C13),+C10/C14,"")</f>
-        <v>0.34883720930232559</v>
+        <v>0.3125</v>
       </c>
       <c r="E10" s="12">
         <v>32000</v>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="D11" s="11">
         <f>IF(SUM(C7:C13),+C11/C14,"")</f>
-        <v>5.8139534883720929E-2</v>
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="E11" s="12">
         <v>6000</v>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="D12" s="11">
         <f>IF(SUM(C7:C13),+C12/C14,"")</f>
-        <v>5.8139534883720929E-2</v>
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="E12" s="12">
         <v>7000</v>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="D13" s="15">
         <f>IF(SUM(C7:C13),+C13/C14,"")</f>
-        <v>1.1627906976744186E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E13" s="14">
         <v>1000</v>
@@ -1872,11 +1872,11 @@
       </c>
       <c r="C14" s="16">
         <f>IF(SUM(C7:C13),SUM(C7:C13),"")</f>
-        <v>86000</v>
+        <v>96000</v>
       </c>
       <c r="D14" s="17">
         <f>IF(SUM(C7:C13),C14/C49,"")</f>
-        <v>0.11894882434301521</v>
+        <v>0.13096862210095497</v>
       </c>
       <c r="E14" s="16">
         <f>IF(SUM(E7:E13),SUM(E7:E13),"")</f>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="D19" s="17">
         <f>IF(SUM(C16:C18),+C19/C49,"")</f>
-        <v>1.7980636237897647E-2</v>
+        <v>1.7735334242837655E-2</v>
       </c>
       <c r="E19" s="16">
         <f>IF(SUM(E16:E18),SUM(E16:E18),"")</f>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="D27" s="17">
         <f>IF(SUM(C21:C26),C27/C49,"")</f>
-        <v>0.50345781466113415</v>
+        <v>0.49658935879945432</v>
       </c>
       <c r="E27" s="16">
         <f>IF(SUM(E21:E26),SUM(E21:E26),"")</f>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="D33" s="17">
         <f>IF(SUM(C29:C32),+C33/C49,"")</f>
-        <v>6.3623789764868599E-2</v>
+        <v>6.2755798090040935E-2</v>
       </c>
       <c r="E33" s="16">
         <f>IF(SUM(E29:E32),SUM(E29:E32),"")</f>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="D41" s="17">
         <f>IF(SUM(C35:C40),+C41/C49,"")</f>
-        <v>0.2544951590594744</v>
+        <v>0.25102319236016374</v>
       </c>
       <c r="E41" s="16">
         <f>IF(SUM(E35:E40),SUM(E35:E40),"")</f>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="D48" s="17">
         <f>IF(SUM(C43:C47),+C48/C49,"")</f>
-        <v>4.1493775933609957E-2</v>
+        <v>4.0927694406548434E-2</v>
       </c>
       <c r="E48" s="16">
         <f>IF(SUM(E43:E47),SUM(E43:E47),"")</f>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="C49" s="16">
         <f>IF(SUM(C14,C19,C27,C33,C41),SUM(C14,C19,C27,C33,C41,C48),"")</f>
-        <v>723000</v>
+        <v>733000</v>
       </c>
       <c r="D49" s="19">
         <f>IF(SUM(C49),+C49/C49,"")</f>
@@ -2984,15 +2984,15 @@
     </row>
     <row r="50" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="52" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B52" s="21"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>